<commit_message>
add: dist\origin.xlsx - move the service columns (with support type) to the beginning of the table (after the label column).
</commit_message>
<xml_diff>
--- a/dist/origin.xlsx
+++ b/dist/origin.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12045" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12045" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="@core" sheetId="2" r:id="rId1"/>
+    <sheet name="@core" sheetId="4" r:id="rId1"/>
     <sheet name="@examples" sheetId="3" r:id="rId2"/>
+    <sheet name="@examples (2)" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,14 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="92">
   <si>
     <t>Settings</t>
   </si>
   <si>
-    <t>ai_counter_locale_table</t>
-  </si>
-  <si>
     <t>show_lid_columns</t>
   </si>
   <si>
@@ -63,6 +61,9 @@
     <t>note:ltext</t>
   </si>
   <si>
+    <t>sig:formula</t>
+  </si>
+  <si>
     <t>type:ref</t>
   </si>
   <si>
@@ -87,7 +88,223 @@
     <t>grass.glb</t>
   </si>
   <si>
-    <t>sig:formula</t>
+    <t>id:1</t>
+  </si>
+  <si>
+    <t>sig:support</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>id:3</t>
+  </si>
+  <si>
+    <t>1: ENTITY_35-1-1-1</t>
+  </si>
+  <si>
+    <t>ENTITY_1</t>
+  </si>
+  <si>
+    <t>2: ENTITY_35-1-1-1</t>
+  </si>
+  <si>
+    <t>ENTITY_2</t>
+  </si>
+  <si>
+    <t>ENTITY_35-1-1-1</t>
+  </si>
+  <si>
+    <t>ENTITY_14</t>
+  </si>
+  <si>
+    <t>ENTITY_6</t>
+  </si>
+  <si>
+    <t>ENTITY_7</t>
+  </si>
+  <si>
+    <t>ENTITY_8</t>
+  </si>
+  <si>
+    <t>ENTITY_9</t>
+  </si>
+  <si>
+    <t>ENTITY_10</t>
+  </si>
+  <si>
+    <t>ENTITY_11</t>
+  </si>
+  <si>
+    <t>ENTITY_12</t>
+  </si>
+  <si>
+    <t>ENTITY_13</t>
+  </si>
+  <si>
+    <t>ENTITY_15</t>
+  </si>
+  <si>
+    <t>ENTITY_16</t>
+  </si>
+  <si>
+    <t>ENTITY_17</t>
+  </si>
+  <si>
+    <t>ENTITY_18</t>
+  </si>
+  <si>
+    <t>ENTITY_19</t>
+  </si>
+  <si>
+    <t>ENTITY_20</t>
+  </si>
+  <si>
+    <t>ENTITY_21</t>
+  </si>
+  <si>
+    <t>ENTITY_22</t>
+  </si>
+  <si>
+    <t>ENTITY_35-1-1-135</t>
+  </si>
+  <si>
+    <t>ENTITY_42</t>
+  </si>
+  <si>
+    <t>ENTITY_43</t>
+  </si>
+  <si>
+    <t>ENTITY_44</t>
+  </si>
+  <si>
+    <t>ENTITY_45</t>
+  </si>
+  <si>
+    <t>ENTITY_46</t>
+  </si>
+  <si>
+    <t>ENTITY_69</t>
+  </si>
+  <si>
+    <t>ENTITY_70</t>
+  </si>
+  <si>
+    <t>ENTITY_71</t>
+  </si>
+  <si>
+    <t>ENTITY_74</t>
+  </si>
+  <si>
+    <t>ENTITY_76</t>
+  </si>
+  <si>
+    <t>ENTITY_72</t>
+  </si>
+  <si>
+    <t>ENTITY_73</t>
+  </si>
+  <si>
+    <t>ENTITY_80</t>
+  </si>
+  <si>
+    <t>ENTITY_78</t>
+  </si>
+  <si>
+    <t>ENTITY_79</t>
+  </si>
+  <si>
+    <t>ENTITY_82</t>
+  </si>
+  <si>
+    <t>ENTITY_92</t>
+  </si>
+  <si>
+    <t>ENTITY_81</t>
+  </si>
+  <si>
+    <t>ENTITY_84</t>
+  </si>
+  <si>
+    <t>ENTITY_86</t>
+  </si>
+  <si>
+    <t>ENTITY_87</t>
+  </si>
+  <si>
+    <t>ENTITY_88</t>
+  </si>
+  <si>
+    <t>ENTITY_89</t>
+  </si>
+  <si>
+    <t>ENTITY_90</t>
+  </si>
+  <si>
+    <t>ENTITY_100</t>
+  </si>
+  <si>
+    <t>ENTITY_102</t>
+  </si>
+  <si>
+    <t>ENTITY_103</t>
+  </si>
+  <si>
+    <t>ENTITY_104</t>
+  </si>
+  <si>
+    <t>ENTITY_105</t>
+  </si>
+  <si>
+    <t>ENTITY_106</t>
+  </si>
+  <si>
+    <t>ENTITY_108</t>
+  </si>
+  <si>
+    <t>ENTITY_109</t>
+  </si>
+  <si>
+    <t>ENTITY_110</t>
+  </si>
+  <si>
+    <t>ENTITY_111</t>
+  </si>
+  <si>
+    <t>ENTITY_112</t>
+  </si>
+  <si>
+    <t>ENTITY_114</t>
+  </si>
+  <si>
+    <t>ENTITY_116</t>
+  </si>
+  <si>
+    <t>ENTITY_118</t>
+  </si>
+  <si>
+    <t>ENTITY_120</t>
+  </si>
+  <si>
+    <t>ENTITY_122</t>
+  </si>
+  <si>
+    <t>ENTITY_124</t>
+  </si>
+  <si>
+    <t>ENTITY_125</t>
+  </si>
+  <si>
+    <t>ENTITY_126</t>
   </si>
 </sst>
 </file>
@@ -703,21 +920,27 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" quotePrefix="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -771,7 +994,118 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="36">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -965,25 +1299,25 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="25"/>
+      <tableStyleElement type="headerRow" dxfId="24"/>
+      <tableStyleElement type="totalRow" dxfId="23"/>
+      <tableStyleElement type="firstColumn" dxfId="22"/>
+      <tableStyleElement type="lastColumn" dxfId="21"/>
+      <tableStyleElement type="firstRowStripe" dxfId="20"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
-      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="35"/>
+      <tableStyleElement type="totalRow" dxfId="34"/>
+      <tableStyleElement type="firstRowStripe" dxfId="33"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="32"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="31"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="30"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="29"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="28"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="27"/>
+      <tableStyleElement type="pageFieldValues" dxfId="26"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -995,20 +1329,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="settings" displayName="settings" ref="B3:C4" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="B3:C4" etc:filterBottomFollowUsedRange="0"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="ai_counter_locale_table"/>
-    <tableColumn id="2" name="show_lid_columns"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="locale" displayName="locale" ref="B9:B10" insertRow="1" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="B9:B10" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="id:0"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="example_base" displayName="example_base" ref="A9:I10" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A9:I10" etc:filterBottomFollowUsedRange="0"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="settings" displayName="settings" ref="B3:B4" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="B3:B4" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="show_lid_columns"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="example_ext_old" displayName="example_ext_old" ref="A2:K3" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A2:K3" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="id:0"/>
     <tableColumn id="2" name="label:label"/>
     <tableColumn id="3" name="name:lid"/>
@@ -1017,19 +1360,59 @@
     <tableColumn id="6" name="desc:ltext"/>
     <tableColumn id="7" name="note:lid"/>
     <tableColumn id="8" name="note:ltext"/>
-    <tableColumn id="9" name="sig:formula">
-      <calculatedColumnFormula>_xlfn.CONCAT(A10,": ",B10)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="11" name="sig:formula" dataDxfId="0"/>
+    <tableColumn id="9" name="type:ref"/>
+    <tableColumn id="10" name="model:text"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="example_ext" displayName="example_ext" ref="A2:J3" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A2:J3" etc:filterBottomFollowUsedRange="0"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="NewTable7" displayName="NewTable7" ref="A6:I7" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A6:I7" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:1" dataDxfId="1"/>
+    <tableColumn id="2" name="label:label" dataDxfId="2"/>
+    <tableColumn id="3" name="sig:support" dataDxfId="3">
+      <calculatedColumnFormula>_xlfn.CONCAT(A7," : ",B7)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid" dataDxfId="4"/>
+    <tableColumn id="5" name="desc:lid" dataDxfId="5"/>
+    <tableColumn id="6" name="note:lid" dataDxfId="6"/>
+    <tableColumn id="7" name="name:ltext" dataDxfId="7"/>
+    <tableColumn id="8" name="desc:ltext" dataDxfId="8"/>
+    <tableColumn id="9" name="note:ltext" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="table_ext" displayName="table_ext" ref="A9:I10" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A9:I10" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:1" dataDxfId="10"/>
+    <tableColumn id="2" name="label:label" dataDxfId="11"/>
+    <tableColumn id="3" name="sig:support" dataDxfId="12">
+      <calculatedColumnFormula>_xlfn.CONCAT(A10," : ",B10)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid" dataDxfId="13"/>
+    <tableColumn id="5" name="desc:lid" dataDxfId="14"/>
+    <tableColumn id="6" name="note:lid" dataDxfId="15"/>
+    <tableColumn id="7" name="name:ltext" dataDxfId="16"/>
+    <tableColumn id="8" name="desc:ltext" dataDxfId="17"/>
+    <tableColumn id="9" name="note:ltext" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="example_extended" displayName="example_extended" ref="A2:J5" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A2:J5" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="id:0"/>
+    <tableColumn id="1" name="id:3"/>
     <tableColumn id="2" name="label:label"/>
     <tableColumn id="3" name="name:lid"/>
     <tableColumn id="4" name="name:ltext"/>
@@ -1037,10 +1420,30 @@
     <tableColumn id="6" name="desc:ltext"/>
     <tableColumn id="7" name="note:lid"/>
     <tableColumn id="8" name="note:ltext"/>
-    <tableColumn id="9" name="type:ref"/>
-    <tableColumn id="10" name="model:text"/>
+    <tableColumn id="9" name="sig:formula">
+      <calculatedColumnFormula>_xlfn.CONCAT(A3,": ",B3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="type:ref"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="example_base8" displayName="example_base8" ref="A8:I81">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A8:I81" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:0" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="label:label"/>
+    <tableColumn id="3" name="name:lid"/>
+    <tableColumn id="4" name="name:ltext"/>
+    <tableColumn id="5" name="desc:lid"/>
+    <tableColumn id="6" name="desc:ltext"/>
+    <tableColumn id="7" name="note:lid"/>
+    <tableColumn id="8" name="note:ltext"/>
+    <tableColumn id="9" name="sig:formula" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1301,41 +1704,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:C4"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="1"/>
-    <col min="2" max="3" width="25.7142857142857" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.4285714285714" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.14285714285714" style="1"/>
+    <col min="2" max="3" width="25.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="24.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1344,8 +1744,9 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1353,154 +1754,2468 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:J10"/>
+  <dimension ref="A2:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7142857142857" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7142857142857" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.14285714285714" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7142857142857" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.14285714285714" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="50.7142857142857" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.14285714285714" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="50.7142857142857" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.7142857142857" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="25.7142857142857" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.14285714285714" style="1"/>
+    <col min="1" max="1" width="10.7142857142857" style="2" customWidth="1"/>
+    <col min="2" max="3" width="25.7142857142857" style="2" customWidth="1"/>
+    <col min="4" max="6" width="10.7142857142857" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.7142857142857" style="2" customWidth="1"/>
+    <col min="8" max="9" width="50.7142857142857" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.7142857142857" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="9.14285714285714" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="str">
+        <f>_xlfn.CONCAT(A3,": ",B3)</f>
+        <v>0: ENTITY_</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f>_xlfn.CONCAT(A7," : ",B7)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f>_xlfn.CONCAT(A10," : ",B10)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A2:J81"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="25.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="9.14285714285714" customWidth="1"/>
+    <col min="4" max="4" width="25.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="9.14285714285714" customWidth="1"/>
+    <col min="6" max="6" width="50.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="9.14285714285714" customWidth="1"/>
+    <col min="8" max="8" width="50.7142857142857" customWidth="1"/>
+    <col min="9" max="10" width="25.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>_xlfn.CONCAT(A3,": ",B3)</f>
+        <v>0: ENTITY_</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>420</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>421</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>422</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" ref="I4:I31" si="0">_xlfn.CONCAT(A4,": ",B4)</f>
+        <v>1: ENTITY_1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2: ENTITY_2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>115</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>116</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>117</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0: ENTITY_</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>118</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>119</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <v>120</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1: ENTITY_35-1-1-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>121</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>122</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>123</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2: ENTITY_35-1-1-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>124</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>125</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12">
+        <v>126</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3: ENTITY_35-1-1-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>127</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>128</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <v>129</v>
+      </c>
+      <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>4: ENTITY_35-1-1-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>130</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>131</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14">
+        <v>132</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>5: ENTITY_35-1-1-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15">
+        <v>42</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f>_xlfn.CONCAT(A15,": ",B15)</f>
+        <v>14: ENTITY_14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f>_xlfn.CONCAT(A16,": ",B16)</f>
+        <v>6: ENTITY_6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17">
+        <v>21</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f>_xlfn.CONCAT(A17,": ",B17)</f>
+        <v>7: ENTITY_7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18">
+        <v>24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f>_xlfn.CONCAT(A18,": ",B18)</f>
+        <v>8: ENTITY_8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19">
+        <v>27</v>
+      </c>
+      <c r="H19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f>_xlfn.CONCAT(A19,": ",B19)</f>
+        <v>9: ENTITY_9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>29</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20">
+        <v>30</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f>_xlfn.CONCAT(A20,": ",B20)</f>
+        <v>10: ENTITY_10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f>_xlfn.CONCAT(A21,": ",B21)</f>
+        <v>11: ENTITY_11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22">
+        <v>36</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f>_xlfn.CONCAT(A22,": ",B22)</f>
+        <v>12: ENTITY_12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
         <v>13</v>
       </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23">
+        <v>38</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23">
+        <v>39</v>
+      </c>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f>_xlfn.CONCAT(A23,": ",B23)</f>
+        <v>13: ENTITY_13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24">
+        <v>45</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>15: ENTITY_15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25">
+        <v>47</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25">
+        <v>48</v>
+      </c>
+      <c r="H25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>16: ENTITY_16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
         <v>17</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26">
+        <v>50</v>
+      </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26">
+        <v>51</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>17: ENTITY_17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>52</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27">
+        <v>53</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <v>54</v>
+      </c>
+      <c r="H27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>18: ENTITY_18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28">
+        <v>56</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28">
+        <v>57</v>
+      </c>
+      <c r="H28" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>19: ENTITY_19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29">
+        <v>58</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29">
+        <v>59</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29">
+        <v>60</v>
+      </c>
+      <c r="H29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>20: ENTITY_20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30">
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30">
+        <v>62</v>
+      </c>
+      <c r="F30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30">
+        <v>63</v>
+      </c>
+      <c r="H30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>21: ENTITY_21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31">
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31">
+        <v>65</v>
+      </c>
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31">
+        <v>66</v>
+      </c>
+      <c r="H31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>22: ENTITY_22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32">
+        <v>217</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32">
+        <v>218</v>
+      </c>
+      <c r="F32" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32">
+        <v>219</v>
+      </c>
+      <c r="H32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33">
+        <v>236</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33">
+        <v>237</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33">
+        <v>238</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34">
+        <v>239</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34">
+        <v>240</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34">
+        <v>241</v>
+      </c>
+      <c r="H34" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35">
+        <v>242</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35">
+        <v>243</v>
+      </c>
+      <c r="F35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35">
+        <v>244</v>
+      </c>
+      <c r="H35" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36">
+        <v>245</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36">
+        <v>246</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36">
+        <v>247</v>
+      </c>
+      <c r="H36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37">
+        <v>248</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37">
+        <v>249</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37">
+        <v>250</v>
+      </c>
+      <c r="H37" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38">
+        <v>62</v>
+      </c>
+      <c r="B38">
+        <v>62</v>
+      </c>
+      <c r="C38">
+        <v>288</v>
+      </c>
+      <c r="E38">
+        <v>289</v>
+      </c>
+      <c r="G38">
+        <v>290</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39">
+        <v>63</v>
+      </c>
+      <c r="B39">
+        <v>63</v>
+      </c>
+      <c r="C39">
+        <v>291</v>
+      </c>
+      <c r="E39">
+        <v>292</v>
+      </c>
+      <c r="G39">
+        <v>293</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40">
+        <v>64</v>
+      </c>
+      <c r="B40">
+        <v>64</v>
+      </c>
+      <c r="C40">
+        <v>294</v>
+      </c>
+      <c r="E40">
+        <v>295</v>
+      </c>
+      <c r="G40">
+        <v>296</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41">
+        <v>65</v>
+      </c>
+      <c r="B41">
+        <v>65</v>
+      </c>
+      <c r="C41">
+        <v>297</v>
+      </c>
+      <c r="E41">
+        <v>298</v>
+      </c>
+      <c r="G41">
+        <v>299</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42">
+        <v>66</v>
+      </c>
+      <c r="B42">
+        <v>66</v>
+      </c>
+      <c r="C42">
+        <v>300</v>
+      </c>
+      <c r="E42">
+        <v>301</v>
+      </c>
+      <c r="G42">
+        <v>302</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43">
+        <v>67</v>
+      </c>
+      <c r="B43">
+        <v>67</v>
+      </c>
+      <c r="C43">
+        <v>303</v>
+      </c>
+      <c r="E43">
+        <v>304</v>
+      </c>
+      <c r="G43">
+        <v>305</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44">
+        <v>69</v>
+      </c>
+      <c r="B44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44">
+        <v>307</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44">
+        <v>308</v>
+      </c>
+      <c r="F44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44">
+        <v>309</v>
+      </c>
+      <c r="H44" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45">
+        <v>70</v>
+      </c>
+      <c r="B45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45">
+        <v>310</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45">
+        <v>311</v>
+      </c>
+      <c r="F45" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45">
+        <v>312</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="1" t="str">
+        <f t="shared" ref="I45:I49" si="1">_xlfn.CONCAT(A45,": ",B45)</f>
+        <v>70: ENTITY_70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46">
+        <v>71</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46">
+        <v>313</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46">
+        <v>314</v>
+      </c>
+      <c r="F46" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46">
+        <v>315</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>71: ENTITY_71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47">
+        <v>74</v>
+      </c>
+      <c r="B47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47">
+        <v>322</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47">
+        <v>323</v>
+      </c>
+      <c r="F47" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47">
+        <v>324</v>
+      </c>
+      <c r="H47" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48">
+        <v>76</v>
+      </c>
+      <c r="B48" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48">
+        <v>326</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48">
+        <v>327</v>
+      </c>
+      <c r="F48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48">
+        <v>328</v>
+      </c>
+      <c r="H48" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49">
+        <v>72</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49">
+        <v>316</v>
+      </c>
+      <c r="D49" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49">
+        <v>317</v>
+      </c>
+      <c r="F49" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49">
+        <v>318</v>
+      </c>
+      <c r="H49" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>72: ENTITY_72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50">
+        <v>73</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50">
+        <v>319</v>
+      </c>
+      <c r="D50" t="s">
+        <v>14</v>
+      </c>
+      <c r="E50">
+        <v>320</v>
+      </c>
+      <c r="F50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50">
+        <v>321</v>
+      </c>
+      <c r="H50" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51">
+        <v>336</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51">
+        <v>337</v>
+      </c>
+      <c r="F51" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51">
+        <v>338</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52">
+        <v>78</v>
+      </c>
+      <c r="B52" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52">
+        <v>330</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52">
+        <v>331</v>
+      </c>
+      <c r="F52" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52">
+        <v>332</v>
+      </c>
+      <c r="H52" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53">
+        <v>79</v>
+      </c>
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53">
+        <v>333</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53">
+        <v>334</v>
+      </c>
+      <c r="F53" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53">
+        <v>335</v>
+      </c>
+      <c r="H53" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54">
+        <v>82</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54">
+        <v>342</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54">
+        <v>343</v>
+      </c>
+      <c r="F54" t="s">
+        <v>15</v>
+      </c>
+      <c r="G54">
+        <v>344</v>
+      </c>
+      <c r="H54" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55">
+        <v>92</v>
+      </c>
+      <c r="B55" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55">
+        <v>366</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55">
+        <v>367</v>
+      </c>
+      <c r="F55" t="s">
+        <v>15</v>
+      </c>
+      <c r="G55">
+        <v>368</v>
+      </c>
+      <c r="H55" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="1" t="str">
+        <f>_xlfn.CONCAT(A55,": ",B55)</f>
+        <v>92: ENTITY_92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56">
+        <v>81</v>
+      </c>
+      <c r="B56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56">
+        <v>339</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56">
+        <v>340</v>
+      </c>
+      <c r="F56" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56">
+        <v>341</v>
+      </c>
+      <c r="H56" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57">
+        <v>84</v>
+      </c>
+      <c r="B57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57">
+        <v>346</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57">
+        <v>347</v>
+      </c>
+      <c r="F57" t="s">
+        <v>15</v>
+      </c>
+      <c r="G57">
+        <v>348</v>
+      </c>
+      <c r="H57" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58">
+        <v>86</v>
+      </c>
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58">
+        <v>350</v>
+      </c>
+      <c r="E58">
+        <v>351</v>
+      </c>
+      <c r="G58">
+        <v>352</v>
+      </c>
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59">
+        <v>87</v>
+      </c>
+      <c r="B59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59">
+        <v>353</v>
+      </c>
+      <c r="E59">
+        <v>354</v>
+      </c>
+      <c r="G59">
+        <v>355</v>
+      </c>
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60">
+        <v>88</v>
+      </c>
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60">
+        <v>356</v>
+      </c>
+      <c r="E60">
+        <v>357</v>
+      </c>
+      <c r="G60">
+        <v>358</v>
+      </c>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61">
+        <v>89</v>
+      </c>
+      <c r="B61" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61">
+        <v>359</v>
+      </c>
+      <c r="E61">
+        <v>360</v>
+      </c>
+      <c r="G61">
+        <v>361</v>
+      </c>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62">
+        <v>90</v>
+      </c>
+      <c r="B62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62">
+        <v>362</v>
+      </c>
+      <c r="E62">
+        <v>363</v>
+      </c>
+      <c r="G62">
+        <v>364</v>
+      </c>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63">
+        <v>100</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63">
+        <v>376</v>
+      </c>
+      <c r="D63" t="s">
+        <v>14</v>
+      </c>
+      <c r="E63">
+        <v>377</v>
+      </c>
+      <c r="F63" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63">
+        <v>378</v>
+      </c>
+      <c r="H63" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" s="1" t="str">
+        <f t="shared" ref="I63:I81" si="2">_xlfn.CONCAT(A63,": ",B63)</f>
+        <v>100: ENTITY_100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64">
+        <v>102</v>
+      </c>
+      <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64">
+        <v>380</v>
+      </c>
+      <c r="D64" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64">
+        <v>381</v>
+      </c>
+      <c r="F64" t="s">
+        <v>15</v>
+      </c>
+      <c r="G64">
+        <v>382</v>
+      </c>
+      <c r="H64" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>102: ENTITY_102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65">
+        <v>103</v>
+      </c>
+      <c r="B65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65">
+        <v>383</v>
+      </c>
+      <c r="D65" t="s">
+        <v>14</v>
+      </c>
+      <c r="E65">
+        <v>384</v>
+      </c>
+      <c r="F65" t="s">
+        <v>15</v>
+      </c>
+      <c r="G65">
+        <v>385</v>
+      </c>
+      <c r="H65" t="s">
+        <v>16</v>
+      </c>
+      <c r="I65" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>103: ENTITY_103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66">
+        <v>104</v>
+      </c>
+      <c r="B66" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66">
+        <v>386</v>
+      </c>
+      <c r="D66" t="s">
+        <v>14</v>
+      </c>
+      <c r="E66">
+        <v>387</v>
+      </c>
+      <c r="F66" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66">
+        <v>388</v>
+      </c>
+      <c r="H66" t="s">
+        <v>16</v>
+      </c>
+      <c r="I66" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>104: ENTITY_104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67">
+        <v>105</v>
+      </c>
+      <c r="B67" t="s">
+        <v>77</v>
+      </c>
+      <c r="C67">
+        <v>389</v>
+      </c>
+      <c r="D67" t="s">
+        <v>14</v>
+      </c>
+      <c r="E67">
+        <v>390</v>
+      </c>
+      <c r="F67" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67">
+        <v>391</v>
+      </c>
+      <c r="H67" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>105: ENTITY_105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68">
+        <v>106</v>
+      </c>
+      <c r="B68" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68">
+        <v>392</v>
+      </c>
+      <c r="D68" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68">
+        <v>393</v>
+      </c>
+      <c r="F68" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68">
+        <v>394</v>
+      </c>
+      <c r="H68" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>106: ENTITY_106</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69">
+        <v>108</v>
+      </c>
+      <c r="B69" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69">
+        <v>396</v>
+      </c>
+      <c r="D69" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69">
+        <v>397</v>
+      </c>
+      <c r="F69" t="s">
+        <v>15</v>
+      </c>
+      <c r="G69">
+        <v>398</v>
+      </c>
+      <c r="H69" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>108: ENTITY_108</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70">
+        <v>109</v>
+      </c>
+      <c r="B70" t="s">
+        <v>80</v>
+      </c>
+      <c r="C70">
+        <v>399</v>
+      </c>
+      <c r="D70" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70">
+        <v>400</v>
+      </c>
+      <c r="F70" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70">
+        <v>401</v>
+      </c>
+      <c r="H70" t="s">
+        <v>16</v>
+      </c>
+      <c r="I70" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>109: ENTITY_109</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71">
+        <v>110</v>
+      </c>
+      <c r="B71" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71">
+        <v>402</v>
+      </c>
+      <c r="D71" t="s">
+        <v>14</v>
+      </c>
+      <c r="E71">
+        <v>403</v>
+      </c>
+      <c r="F71" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71">
+        <v>404</v>
+      </c>
+      <c r="H71" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>110: ENTITY_110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72">
+        <v>111</v>
+      </c>
+      <c r="B72" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72">
+        <v>405</v>
+      </c>
+      <c r="D72" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72">
+        <v>406</v>
+      </c>
+      <c r="F72" t="s">
+        <v>15</v>
+      </c>
+      <c r="G72">
+        <v>407</v>
+      </c>
+      <c r="H72" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>111: ENTITY_111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73">
+        <v>112</v>
+      </c>
+      <c r="B73" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73">
+        <v>408</v>
+      </c>
+      <c r="D73" t="s">
+        <v>14</v>
+      </c>
+      <c r="E73">
+        <v>409</v>
+      </c>
+      <c r="F73" t="s">
+        <v>15</v>
+      </c>
+      <c r="G73">
+        <v>410</v>
+      </c>
+      <c r="H73" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>112: ENTITY_112</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74">
+        <v>114</v>
+      </c>
+      <c r="B74" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74">
+        <v>412</v>
+      </c>
+      <c r="D74" t="s">
+        <v>14</v>
+      </c>
+      <c r="E74">
+        <v>413</v>
+      </c>
+      <c r="F74" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74">
+        <v>414</v>
+      </c>
+      <c r="H74" t="s">
+        <v>16</v>
+      </c>
+      <c r="I74" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>114: ENTITY_114</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75">
+        <v>116</v>
+      </c>
+      <c r="B75" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75">
+        <v>416</v>
+      </c>
+      <c r="D75" t="s">
+        <v>14</v>
+      </c>
+      <c r="E75">
+        <v>417</v>
+      </c>
+      <c r="F75" t="s">
+        <v>15</v>
+      </c>
+      <c r="G75">
+        <v>418</v>
+      </c>
+      <c r="H75" t="s">
+        <v>16</v>
+      </c>
+      <c r="I75" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>116: ENTITY_116</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76">
+        <v>118</v>
+      </c>
+      <c r="B76" t="s">
+        <v>86</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>14</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+      <c r="F76" t="s">
+        <v>15</v>
+      </c>
+      <c r="G76">
         <v>3</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="H76" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>118: ENTITY_118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77">
+        <v>120</v>
+      </c>
+      <c r="B77" t="s">
+        <v>87</v>
+      </c>
+      <c r="C77">
         <v>5</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D77" t="s">
+        <v>14</v>
+      </c>
+      <c r="E77">
         <v>6</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F77" t="s">
+        <v>15</v>
+      </c>
+      <c r="G77">
         <v>7</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="H77" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>120: ENTITY_120</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78">
+        <v>122</v>
+      </c>
+      <c r="B78" t="s">
+        <v>88</v>
+      </c>
+      <c r="C78">
         <v>9</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="D78" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78">
         <v>10</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="F78" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78">
+        <v>11</v>
+      </c>
+      <c r="H78" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>122: ENTITY_122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79">
+        <v>124</v>
+      </c>
+      <c r="B79" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79">
+        <v>13</v>
+      </c>
+      <c r="D79" t="s">
+        <v>14</v>
+      </c>
+      <c r="E79">
+        <v>14</v>
+      </c>
+      <c r="F79" t="s">
+        <v>15</v>
+      </c>
+      <c r="G79">
+        <v>15</v>
+      </c>
+      <c r="H79" t="s">
+        <v>16</v>
+      </c>
+      <c r="I79" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>124: ENTITY_124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80">
+        <v>125</v>
+      </c>
+      <c r="B80" t="s">
+        <v>90</v>
+      </c>
+      <c r="C80">
+        <v>16</v>
+      </c>
+      <c r="D80" t="s">
+        <v>14</v>
+      </c>
+      <c r="E80">
+        <v>17</v>
+      </c>
+      <c r="F80" t="s">
+        <v>15</v>
+      </c>
+      <c r="G80">
+        <v>18</v>
+      </c>
+      <c r="H80" t="s">
+        <v>16</v>
+      </c>
+      <c r="I80" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>125: ENTITY_125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81">
+        <v>126</v>
+      </c>
+      <c r="B81" t="s">
+        <v>91</v>
+      </c>
+      <c r="C81">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="2" t="str">
-        <f>_xlfn.CONCAT(A10,": ",B10)</f>
-        <v>0: ENTITY_</v>
+      <c r="D81" t="s">
+        <v>14</v>
+      </c>
+      <c r="E81">
+        <v>20</v>
+      </c>
+      <c r="F81" t="s">
+        <v>15</v>
+      </c>
+      <c r="G81">
+        <v>21</v>
+      </c>
+      <c r="H81" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>126: ENTITY_126</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3">
-      <formula1>$I$10:$I$10</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J5">
+      <formula1>$I$9:$I$81</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update: dist\origin.xlsx - cleanup.
</commit_message>
<xml_diff>
--- a/dist/origin.xlsx
+++ b/dist/origin.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12045" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="11835" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="@core" sheetId="4" r:id="rId1"/>
     <sheet name="@examples" sheetId="3" r:id="rId2"/>
     <sheet name="@examples (2)" sheetId="5" r:id="rId3"/>
+    <sheet name="NewTable" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="92">
   <si>
     <t>Settings</t>
   </si>
@@ -40,39 +41,60 @@
     <t>id:0</t>
   </si>
   <si>
+    <t>id:1</t>
+  </si>
+  <si>
     <t>label:label</t>
   </si>
   <si>
+    <t>sig:support</t>
+  </si>
+  <si>
     <t>name:lid</t>
   </si>
   <si>
+    <t>desc:lid</t>
+  </si>
+  <si>
+    <t>note:lid</t>
+  </si>
+  <si>
     <t>name:ltext</t>
   </si>
   <si>
-    <t>desc:lid</t>
-  </si>
-  <si>
     <t>desc:ltext</t>
   </si>
   <si>
-    <t>note:lid</t>
-  </si>
-  <si>
     <t>note:ltext</t>
   </si>
   <si>
+    <t>type:ref</t>
+  </si>
+  <si>
+    <t>ENTITY_</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>0 : ENTITY_</t>
+  </si>
+  <si>
+    <t>id:3</t>
+  </si>
+  <si>
     <t>sig:formula</t>
   </si>
   <si>
-    <t>type:ref</t>
-  </si>
-  <si>
-    <t>model:text</t>
-  </si>
-  <si>
-    <t>ENTITY_</t>
-  </si>
-  <si>
     <t>Имя</t>
   </si>
   <si>
@@ -82,102 +104,78 @@
     <t>Примечание</t>
   </si>
   <si>
+    <t>1: ENTITY_35-1-1-1</t>
+  </si>
+  <si>
+    <t>ENTITY_1</t>
+  </si>
+  <si>
+    <t>2: ENTITY_35-1-1-1</t>
+  </si>
+  <si>
+    <t>ENTITY_2</t>
+  </si>
+  <si>
+    <t>ENTITY_35-1-1-1</t>
+  </si>
+  <si>
+    <t>ENTITY_14</t>
+  </si>
+  <si>
+    <t>ENTITY_6</t>
+  </si>
+  <si>
+    <t>ENTITY_7</t>
+  </si>
+  <si>
+    <t>ENTITY_8</t>
+  </si>
+  <si>
+    <t>ENTITY_9</t>
+  </si>
+  <si>
+    <t>ENTITY_10</t>
+  </si>
+  <si>
+    <t>ENTITY_11</t>
+  </si>
+  <si>
+    <t>ENTITY_12</t>
+  </si>
+  <si>
+    <t>ENTITY_13</t>
+  </si>
+  <si>
+    <t>ENTITY_15</t>
+  </si>
+  <si>
+    <t>ENTITY_16</t>
+  </si>
+  <si>
+    <t>ENTITY_17</t>
+  </si>
+  <si>
+    <t>ENTITY_18</t>
+  </si>
+  <si>
+    <t>ENTITY_19</t>
+  </si>
+  <si>
+    <t>ENTITY_20</t>
+  </si>
+  <si>
+    <t>ENTITY_21</t>
+  </si>
+  <si>
+    <t>ENTITY_22</t>
+  </si>
+  <si>
+    <t>ENTITY_35-1-1-135</t>
+  </si>
+  <si>
     <t>0: ENTITY_</t>
   </si>
   <si>
-    <t>grass.glb</t>
-  </si>
-  <si>
-    <t>id:1</t>
-  </si>
-  <si>
-    <t>sig:support</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>id:3</t>
-  </si>
-  <si>
-    <t>1: ENTITY_35-1-1-1</t>
-  </si>
-  <si>
-    <t>ENTITY_1</t>
-  </si>
-  <si>
-    <t>2: ENTITY_35-1-1-1</t>
-  </si>
-  <si>
-    <t>ENTITY_2</t>
-  </si>
-  <si>
-    <t>ENTITY_35-1-1-1</t>
-  </si>
-  <si>
-    <t>ENTITY_14</t>
-  </si>
-  <si>
-    <t>ENTITY_6</t>
-  </si>
-  <si>
-    <t>ENTITY_7</t>
-  </si>
-  <si>
-    <t>ENTITY_8</t>
-  </si>
-  <si>
-    <t>ENTITY_9</t>
-  </si>
-  <si>
-    <t>ENTITY_10</t>
-  </si>
-  <si>
-    <t>ENTITY_11</t>
-  </si>
-  <si>
-    <t>ENTITY_12</t>
-  </si>
-  <si>
-    <t>ENTITY_13</t>
-  </si>
-  <si>
-    <t>ENTITY_15</t>
-  </si>
-  <si>
-    <t>ENTITY_16</t>
-  </si>
-  <si>
-    <t>ENTITY_17</t>
-  </si>
-  <si>
-    <t>ENTITY_18</t>
-  </si>
-  <si>
-    <t>ENTITY_19</t>
-  </si>
-  <si>
-    <t>ENTITY_20</t>
-  </si>
-  <si>
-    <t>ENTITY_21</t>
-  </si>
-  <si>
-    <t>ENTITY_22</t>
-  </si>
-  <si>
-    <t>ENTITY_35-1-1-135</t>
-  </si>
-  <si>
     <t>ENTITY_42</t>
   </si>
   <si>
@@ -305,6 +303,9 @@
   </si>
   <si>
     <t>ENTITY_126</t>
+  </si>
+  <si>
+    <t>signature:support</t>
   </si>
 </sst>
 </file>
@@ -920,7 +921,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -928,9 +929,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -940,6 +938,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -994,10 +995,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="35">
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -1299,25 +1297,25 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="25"/>
-      <tableStyleElement type="headerRow" dxfId="24"/>
-      <tableStyleElement type="totalRow" dxfId="23"/>
-      <tableStyleElement type="firstColumn" dxfId="22"/>
-      <tableStyleElement type="lastColumn" dxfId="21"/>
-      <tableStyleElement type="firstRowStripe" dxfId="20"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="19"/>
+      <tableStyleElement type="wholeTable" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="totalRow" dxfId="22"/>
+      <tableStyleElement type="firstColumn" dxfId="21"/>
+      <tableStyleElement type="lastColumn" dxfId="20"/>
+      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="18"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="35"/>
-      <tableStyleElement type="totalRow" dxfId="34"/>
-      <tableStyleElement type="firstRowStripe" dxfId="33"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="32"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="31"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="30"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="29"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="28"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="27"/>
-      <tableStyleElement type="pageFieldValues" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="34"/>
+      <tableStyleElement type="totalRow" dxfId="33"/>
+      <tableStyleElement type="firstRowStripe" dxfId="32"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="31"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="30"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="29"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="28"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="27"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="26"/>
+      <tableStyleElement type="pageFieldValues" dxfId="25"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1349,66 +1347,47 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="example_ext_old" displayName="example_ext_old" ref="A2:K3" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A2:K3" etc:filterBottomFollowUsedRange="0"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="id:0"/>
-    <tableColumn id="2" name="label:label"/>
-    <tableColumn id="3" name="name:lid"/>
-    <tableColumn id="4" name="name:ltext"/>
-    <tableColumn id="5" name="desc:lid"/>
-    <tableColumn id="6" name="desc:ltext"/>
-    <tableColumn id="7" name="note:lid"/>
-    <tableColumn id="8" name="note:ltext"/>
-    <tableColumn id="11" name="sig:formula" dataDxfId="0"/>
-    <tableColumn id="9" name="type:ref"/>
-    <tableColumn id="10" name="model:text"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="table_base" displayName="table_base" ref="A2:J3" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A2:J3" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="id:1" dataDxfId="0"/>
+    <tableColumn id="2" name="label:label" dataDxfId="1"/>
+    <tableColumn id="3" name="sig:support" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.CONCAT(A3," : ",B3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid" dataDxfId="3"/>
+    <tableColumn id="5" name="desc:lid" dataDxfId="4"/>
+    <tableColumn id="6" name="note:lid" dataDxfId="5"/>
+    <tableColumn id="7" name="name:ltext" dataDxfId="6"/>
+    <tableColumn id="8" name="desc:ltext" dataDxfId="7"/>
+    <tableColumn id="10" name="note:ltext"/>
+    <tableColumn id="9" name="type:ref" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="NewTable7" displayName="NewTable7" ref="A6:I7" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A6:I7" etc:filterBottomFollowUsedRange="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="table_ext" displayName="table_ext" ref="A5:I6" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A5:I6" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="id:1" dataDxfId="1"/>
-    <tableColumn id="2" name="label:label" dataDxfId="2"/>
-    <tableColumn id="3" name="sig:support" dataDxfId="3">
-      <calculatedColumnFormula>_xlfn.CONCAT(A7," : ",B7)</calculatedColumnFormula>
+    <tableColumn id="1" name="id:1" dataDxfId="9"/>
+    <tableColumn id="2" name="label:label" dataDxfId="10"/>
+    <tableColumn id="3" name="sig:support" dataDxfId="11">
+      <calculatedColumnFormula>_xlfn.CONCAT(A6," : ",B6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="name:lid" dataDxfId="4"/>
-    <tableColumn id="5" name="desc:lid" dataDxfId="5"/>
-    <tableColumn id="6" name="note:lid" dataDxfId="6"/>
-    <tableColumn id="7" name="name:ltext" dataDxfId="7"/>
-    <tableColumn id="8" name="desc:ltext" dataDxfId="8"/>
-    <tableColumn id="9" name="note:ltext" dataDxfId="9"/>
+    <tableColumn id="4" name="name:lid" dataDxfId="12"/>
+    <tableColumn id="5" name="desc:lid" dataDxfId="13"/>
+    <tableColumn id="6" name="note:lid" dataDxfId="14"/>
+    <tableColumn id="7" name="name:ltext" dataDxfId="15"/>
+    <tableColumn id="8" name="desc:ltext" dataDxfId="16"/>
+    <tableColumn id="9" name="note:ltext" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="table_ext" displayName="table_ext" ref="A9:I10" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A9:I10" etc:filterBottomFollowUsedRange="0"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="id:1" dataDxfId="10"/>
-    <tableColumn id="2" name="label:label" dataDxfId="11"/>
-    <tableColumn id="3" name="sig:support" dataDxfId="12">
-      <calculatedColumnFormula>_xlfn.CONCAT(A10," : ",B10)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" name="name:lid" dataDxfId="13"/>
-    <tableColumn id="5" name="desc:lid" dataDxfId="14"/>
-    <tableColumn id="6" name="note:lid" dataDxfId="15"/>
-    <tableColumn id="7" name="name:ltext" dataDxfId="16"/>
-    <tableColumn id="8" name="desc:ltext" dataDxfId="17"/>
-    <tableColumn id="9" name="note:ltext" dataDxfId="18"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="example_extended" displayName="example_extended" ref="A2:J5" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A2:J5" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="10">
@@ -1429,7 +1408,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="example_base8" displayName="example_base8" ref="A8:I81">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A8:I81" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="9">
@@ -1444,6 +1423,26 @@
     <tableColumn id="9" name="sig:formula" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="NewTable" displayName="NewTable" ref="A1:I2" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I2" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:1"/>
+    <tableColumn id="2" name="label:label"/>
+    <tableColumn id="3" name="signature:support">
+      <calculatedColumnFormula>_xlfn.CONCAT(A2," : ",B2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid"/>
+    <tableColumn id="5" name="desc:lid"/>
+    <tableColumn id="6" name="note:lid"/>
+    <tableColumn id="7" name="name:ltext"/>
+    <tableColumn id="8" name="desc:ltext"/>
+    <tableColumn id="9" name="note:ltext"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1708,7 +1707,7 @@
   <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1718,10 +1717,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
@@ -1729,7 +1728,7 @@
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4" s="5" t="b">
+      <c r="B4" s="4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1754,13 +1753,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:K10"/>
+  <dimension ref="A2:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C19" sqref="C18:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="10.7142857142857" style="2" customWidth="1"/>
     <col min="2" max="3" width="25.7142857142857" style="2" customWidth="1"/>
@@ -1771,207 +1770,141 @@
     <col min="11" max="16384" width="9.14285714285714" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:10">
       <c r="A3" s="2">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="2" t="str">
+        <f>_xlfn.CONCAT(A3," : ",B3)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="3" t="str">
-        <f>_xlfn.CONCAT(A3,": ",B3)</f>
-        <v>0: ENTITY_</v>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f>_xlfn.CONCAT(A6," : ",B6)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="2">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="str">
-        <f>_xlfn.CONCAT(A7," : ",B7)</f>
-        <v>0 : ENTITY_</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f>_xlfn.CONCAT(A10," : ",B10)</f>
-        <v>0 : ENTITY_</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3">
-      <formula1>#REF!</formula1>
+      <formula1>$C$6:$C$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
-  <tableParts count="3">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2000,34 +1933,34 @@
   <sheetData>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2041,26 +1974,26 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I3" s="1" t="str">
         <f>_xlfn.CONCAT(A3,": ",B3)</f>
         <v>0: ENTITY_</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2068,32 +2001,32 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>420</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>421</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G4">
         <v>422</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I4" s="1" t="str">
         <f t="shared" ref="I4:I31" si="0">_xlfn.CONCAT(A4,": ",B4)</f>
         <v>1: ENTITY_1</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2101,32 +2034,32 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G5">
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>2: ENTITY_2</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2134,28 +2067,28 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2169,19 +2102,19 @@
         <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G9">
         <v>117</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2193,25 +2126,25 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>118</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E10">
         <v>119</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G10">
         <v>120</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2223,25 +2156,25 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>121</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E11">
         <v>122</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G11">
         <v>123</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2253,25 +2186,25 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>124</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>125</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G12">
         <v>126</v>
       </c>
       <c r="H12" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2283,25 +2216,25 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>127</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>128</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G13">
         <v>129</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2313,25 +2246,25 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>130</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>131</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G14">
         <v>132</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2343,25 +2276,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E15">
         <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G15">
         <v>42</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I15" s="1" t="str">
         <f>_xlfn.CONCAT(A15,": ",B15)</f>
@@ -2373,25 +2306,25 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E16">
         <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G16">
         <v>18</v>
       </c>
       <c r="H16" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I16" s="1" t="str">
         <f>_xlfn.CONCAT(A16,": ",B16)</f>
@@ -2403,25 +2336,25 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E17">
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G17">
         <v>21</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I17" s="1" t="str">
         <f>_xlfn.CONCAT(A17,": ",B17)</f>
@@ -2433,25 +2366,25 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E18">
         <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G18">
         <v>24</v>
       </c>
       <c r="H18" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I18" s="1" t="str">
         <f>_xlfn.CONCAT(A18,": ",B18)</f>
@@ -2463,25 +2396,25 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19">
         <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E19">
         <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G19">
         <v>27</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I19" s="1" t="str">
         <f>_xlfn.CONCAT(A19,": ",B19)</f>
@@ -2493,25 +2426,25 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20">
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E20">
         <v>29</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G20">
         <v>30</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I20" s="1" t="str">
         <f>_xlfn.CONCAT(A20,": ",B20)</f>
@@ -2523,25 +2456,25 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E21">
         <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G21">
         <v>33</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I21" s="1" t="str">
         <f>_xlfn.CONCAT(A21,": ",B21)</f>
@@ -2553,25 +2486,25 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22">
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E22">
         <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G22">
         <v>36</v>
       </c>
       <c r="H22" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I22" s="1" t="str">
         <f>_xlfn.CONCAT(A22,": ",B22)</f>
@@ -2583,25 +2516,25 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23">
         <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E23">
         <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G23">
         <v>39</v>
       </c>
       <c r="H23" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I23" s="1" t="str">
         <f>_xlfn.CONCAT(A23,": ",B23)</f>
@@ -2613,25 +2546,25 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24">
         <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E24">
         <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G24">
         <v>45</v>
       </c>
       <c r="H24" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2643,25 +2576,25 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C25">
         <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E25">
         <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G25">
         <v>48</v>
       </c>
       <c r="H25" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2673,25 +2606,25 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26">
         <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E26">
         <v>50</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G26">
         <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2703,25 +2636,25 @@
         <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27">
         <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E27">
         <v>53</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G27">
         <v>54</v>
       </c>
       <c r="H27" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2733,25 +2666,25 @@
         <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28">
         <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E28">
         <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G28">
         <v>57</v>
       </c>
       <c r="H28" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2763,25 +2696,25 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C29">
         <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E29">
         <v>59</v>
       </c>
       <c r="F29" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G29">
         <v>60</v>
       </c>
       <c r="H29" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2793,25 +2726,25 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30">
         <v>61</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E30">
         <v>62</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G30">
         <v>63</v>
       </c>
       <c r="H30" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2823,25 +2756,25 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31">
         <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E31">
         <v>65</v>
       </c>
       <c r="F31" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G31">
         <v>66</v>
       </c>
       <c r="H31" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2853,28 +2786,28 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C32">
         <v>217</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E32">
         <v>218</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G32">
         <v>219</v>
       </c>
       <c r="H32" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2882,28 +2815,28 @@
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33">
         <v>236</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E33">
         <v>237</v>
       </c>
       <c r="F33" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G33">
         <v>238</v>
       </c>
       <c r="H33" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2911,28 +2844,28 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34">
         <v>239</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E34">
         <v>240</v>
       </c>
       <c r="F34" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G34">
         <v>241</v>
       </c>
       <c r="H34" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2940,28 +2873,28 @@
         <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35">
         <v>242</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E35">
         <v>243</v>
       </c>
       <c r="F35" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G35">
         <v>244</v>
       </c>
       <c r="H35" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2969,28 +2902,28 @@
         <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36">
         <v>245</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E36">
         <v>246</v>
       </c>
       <c r="F36" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G36">
         <v>247</v>
       </c>
       <c r="H36" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2998,28 +2931,28 @@
         <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37">
         <v>248</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E37">
         <v>249</v>
       </c>
       <c r="F37" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G37">
         <v>250</v>
       </c>
       <c r="H37" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -3039,7 +2972,7 @@
         <v>290</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -3059,7 +2992,7 @@
         <v>293</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3079,7 +3012,7 @@
         <v>296</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -3099,7 +3032,7 @@
         <v>299</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3119,7 +3052,7 @@
         <v>302</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3139,7 +3072,7 @@
         <v>305</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3147,28 +3080,28 @@
         <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44">
         <v>307</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E44">
         <v>308</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G44">
         <v>309</v>
       </c>
       <c r="H44" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3176,25 +3109,25 @@
         <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45">
         <v>310</v>
       </c>
       <c r="D45" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E45">
         <v>311</v>
       </c>
       <c r="F45" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G45">
         <v>312</v>
       </c>
       <c r="H45" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I45" s="1" t="str">
         <f t="shared" ref="I45:I49" si="1">_xlfn.CONCAT(A45,": ",B45)</f>
@@ -3206,25 +3139,25 @@
         <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46">
         <v>313</v>
       </c>
       <c r="D46" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E46">
         <v>314</v>
       </c>
       <c r="F46" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G46">
         <v>315</v>
       </c>
       <c r="H46" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I46" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3236,28 +3169,28 @@
         <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47">
         <v>322</v>
       </c>
       <c r="D47" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E47">
         <v>323</v>
       </c>
       <c r="F47" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G47">
         <v>324</v>
       </c>
       <c r="H47" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -3265,28 +3198,28 @@
         <v>76</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48">
         <v>326</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E48">
         <v>327</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G48">
         <v>328</v>
       </c>
       <c r="H48" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3294,25 +3227,25 @@
         <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49">
         <v>316</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E49">
         <v>317</v>
       </c>
       <c r="F49" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G49">
         <v>318</v>
       </c>
       <c r="H49" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I49" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3324,28 +3257,28 @@
         <v>73</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50">
         <v>319</v>
       </c>
       <c r="D50" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E50">
         <v>320</v>
       </c>
       <c r="F50" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G50">
         <v>321</v>
       </c>
       <c r="H50" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -3353,28 +3286,28 @@
         <v>80</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51">
         <v>336</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E51">
         <v>337</v>
       </c>
       <c r="F51" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G51">
         <v>338</v>
       </c>
       <c r="H51" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -3382,28 +3315,28 @@
         <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52">
         <v>330</v>
       </c>
       <c r="D52" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E52">
         <v>331</v>
       </c>
       <c r="F52" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G52">
         <v>332</v>
       </c>
       <c r="H52" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -3411,28 +3344,28 @@
         <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53">
         <v>333</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E53">
         <v>334</v>
       </c>
       <c r="F53" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G53">
         <v>335</v>
       </c>
       <c r="H53" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3440,28 +3373,28 @@
         <v>82</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54">
         <v>342</v>
       </c>
       <c r="D54" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E54">
         <v>343</v>
       </c>
       <c r="F54" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G54">
         <v>344</v>
       </c>
       <c r="H54" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -3469,25 +3402,25 @@
         <v>92</v>
       </c>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55">
         <v>366</v>
       </c>
       <c r="D55" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E55">
         <v>367</v>
       </c>
       <c r="F55" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G55">
         <v>368</v>
       </c>
       <c r="H55" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I55" s="1" t="str">
         <f>_xlfn.CONCAT(A55,": ",B55)</f>
@@ -3499,28 +3432,28 @@
         <v>81</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56">
         <v>339</v>
       </c>
       <c r="D56" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E56">
         <v>340</v>
       </c>
       <c r="F56" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G56">
         <v>341</v>
       </c>
       <c r="H56" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -3528,28 +3461,28 @@
         <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57">
         <v>346</v>
       </c>
       <c r="D57" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E57">
         <v>347</v>
       </c>
       <c r="F57" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G57">
         <v>348</v>
       </c>
       <c r="H57" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -3557,7 +3490,7 @@
         <v>86</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58">
         <v>350</v>
@@ -3575,7 +3508,7 @@
         <v>87</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59">
         <v>353</v>
@@ -3593,7 +3526,7 @@
         <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60">
         <v>356</v>
@@ -3611,7 +3544,7 @@
         <v>89</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C61">
         <v>359</v>
@@ -3629,7 +3562,7 @@
         <v>90</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C62">
         <v>362</v>
@@ -3647,25 +3580,25 @@
         <v>100</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63">
         <v>376</v>
       </c>
       <c r="D63" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E63">
         <v>377</v>
       </c>
       <c r="F63" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G63">
         <v>378</v>
       </c>
       <c r="H63" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I63" s="1" t="str">
         <f t="shared" ref="I63:I81" si="2">_xlfn.CONCAT(A63,": ",B63)</f>
@@ -3677,25 +3610,25 @@
         <v>102</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64">
         <v>380</v>
       </c>
       <c r="D64" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E64">
         <v>381</v>
       </c>
       <c r="F64" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G64">
         <v>382</v>
       </c>
       <c r="H64" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I64" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3707,25 +3640,25 @@
         <v>103</v>
       </c>
       <c r="B65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C65">
         <v>383</v>
       </c>
       <c r="D65" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E65">
         <v>384</v>
       </c>
       <c r="F65" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G65">
         <v>385</v>
       </c>
       <c r="H65" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I65" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3737,25 +3670,25 @@
         <v>104</v>
       </c>
       <c r="B66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C66">
         <v>386</v>
       </c>
       <c r="D66" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E66">
         <v>387</v>
       </c>
       <c r="F66" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G66">
         <v>388</v>
       </c>
       <c r="H66" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I66" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3767,25 +3700,25 @@
         <v>105</v>
       </c>
       <c r="B67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C67">
         <v>389</v>
       </c>
       <c r="D67" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E67">
         <v>390</v>
       </c>
       <c r="F67" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G67">
         <v>391</v>
       </c>
       <c r="H67" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I67" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3797,25 +3730,25 @@
         <v>106</v>
       </c>
       <c r="B68" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68">
         <v>392</v>
       </c>
       <c r="D68" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E68">
         <v>393</v>
       </c>
       <c r="F68" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G68">
         <v>394</v>
       </c>
       <c r="H68" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I68" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3827,25 +3760,25 @@
         <v>108</v>
       </c>
       <c r="B69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C69">
         <v>396</v>
       </c>
       <c r="D69" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E69">
         <v>397</v>
       </c>
       <c r="F69" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G69">
         <v>398</v>
       </c>
       <c r="H69" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I69" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3857,25 +3790,25 @@
         <v>109</v>
       </c>
       <c r="B70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C70">
         <v>399</v>
       </c>
       <c r="D70" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E70">
         <v>400</v>
       </c>
       <c r="F70" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G70">
         <v>401</v>
       </c>
       <c r="H70" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I70" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3887,25 +3820,25 @@
         <v>110</v>
       </c>
       <c r="B71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C71">
         <v>402</v>
       </c>
       <c r="D71" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E71">
         <v>403</v>
       </c>
       <c r="F71" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G71">
         <v>404</v>
       </c>
       <c r="H71" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I71" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3917,25 +3850,25 @@
         <v>111</v>
       </c>
       <c r="B72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C72">
         <v>405</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E72">
         <v>406</v>
       </c>
       <c r="F72" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G72">
         <v>407</v>
       </c>
       <c r="H72" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I72" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3947,25 +3880,25 @@
         <v>112</v>
       </c>
       <c r="B73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C73">
         <v>408</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E73">
         <v>409</v>
       </c>
       <c r="F73" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G73">
         <v>410</v>
       </c>
       <c r="H73" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I73" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3977,25 +3910,25 @@
         <v>114</v>
       </c>
       <c r="B74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C74">
         <v>412</v>
       </c>
       <c r="D74" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E74">
         <v>413</v>
       </c>
       <c r="F74" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G74">
         <v>414</v>
       </c>
       <c r="H74" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I74" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4007,25 +3940,25 @@
         <v>116</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C75">
         <v>416</v>
       </c>
       <c r="D75" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E75">
         <v>417</v>
       </c>
       <c r="F75" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G75">
         <v>418</v>
       </c>
       <c r="H75" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I75" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4037,25 +3970,25 @@
         <v>118</v>
       </c>
       <c r="B76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E76">
         <v>2</v>
       </c>
       <c r="F76" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G76">
         <v>3</v>
       </c>
       <c r="H76" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I76" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4067,25 +4000,25 @@
         <v>120</v>
       </c>
       <c r="B77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C77">
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E77">
         <v>6</v>
       </c>
       <c r="F77" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G77">
         <v>7</v>
       </c>
       <c r="H77" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I77" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4097,25 +4030,25 @@
         <v>122</v>
       </c>
       <c r="B78" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C78">
         <v>9</v>
       </c>
       <c r="D78" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E78">
         <v>10</v>
       </c>
       <c r="F78" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G78">
         <v>11</v>
       </c>
       <c r="H78" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I78" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4127,25 +4060,25 @@
         <v>124</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C79">
         <v>13</v>
       </c>
       <c r="D79" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E79">
         <v>14</v>
       </c>
       <c r="F79" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G79">
         <v>15</v>
       </c>
       <c r="H79" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I79" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4157,25 +4090,25 @@
         <v>125</v>
       </c>
       <c r="B80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C80">
         <v>16</v>
       </c>
       <c r="D80" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E80">
         <v>17</v>
       </c>
       <c r="F80" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G80">
         <v>18</v>
       </c>
       <c r="H80" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I80" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4187,25 +4120,25 @@
         <v>126</v>
       </c>
       <c r="B81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C81">
         <v>19</v>
       </c>
       <c r="D81" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E81">
         <v>20</v>
       </c>
       <c r="F81" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G81">
         <v>21</v>
       </c>
       <c r="H81" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="I81" s="1" t="str">
         <f t="shared" si="2"/>
@@ -4225,4 +4158,90 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="10.7142857142857" customWidth="1"/>
+    <col min="2" max="3" width="25.7142857142857" customWidth="1"/>
+    <col min="4" max="6" width="10.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="25.7142857142857" customWidth="1"/>
+    <col min="8" max="9" width="50.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT(A2," : ",B2)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update: dist\data_designer.xaml - the first row in each table now refers to the locale table.
</commit_message>
<xml_diff>
--- a/dist/origin.xlsx
+++ b/dist/origin.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12045" firstSheet="1"/>
+    <workbookView windowWidth="27945" windowHeight="12045" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="@core" sheetId="4" r:id="rId1"/>
-    <sheet name="@examples" sheetId="3" r:id="rId2"/>
+    <sheet name="NewTable" sheetId="7" r:id="rId2"/>
+    <sheet name="@examples" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="20">
   <si>
     <t>Settings</t>
   </si>
@@ -39,16 +40,13 @@
     <t>show_support_columns</t>
   </si>
   <si>
-    <t>id:0</t>
-  </si>
-  <si>
     <t>id:1</t>
   </si>
   <si>
     <t>label:label</t>
   </si>
   <si>
-    <t>sig:support</t>
+    <t>signature:support</t>
   </si>
   <si>
     <t>name:lid</t>
@@ -69,13 +67,7 @@
     <t>note:ltext</t>
   </si>
   <si>
-    <t>type:ref</t>
-  </si>
-  <si>
     <t>ENTITY_</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Name</t>
@@ -85,6 +77,15 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>sig:support</t>
+  </si>
+  <si>
+    <t>type:ref</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>0 : ENTITY_</t>
@@ -1106,7 +1107,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="locale" displayName="locale" ref="B9:B10" insertRow="1" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="B9:B10" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="id:0"/>
+    <tableColumn id="1" name="id:1"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1124,6 +1125,66 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="NewTable" displayName="NewTable" ref="A1:I2" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I2" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:1"/>
+    <tableColumn id="2" name="label:label"/>
+    <tableColumn id="3" name="signature:support">
+      <calculatedColumnFormula>_xlfn.CONCAT(A2," : ",B2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid"/>
+    <tableColumn id="5" name="desc:lid"/>
+    <tableColumn id="6" name="note:lid"/>
+    <tableColumn id="7" name="name:ltext"/>
+    <tableColumn id="8" name="desc:ltext"/>
+    <tableColumn id="9" name="note:ltext"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="NewTabley" displayName="NewTabley" ref="A4:I5" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A4:I5" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:1"/>
+    <tableColumn id="2" name="label:label"/>
+    <tableColumn id="3" name="signature:support">
+      <calculatedColumnFormula>_xlfn.CONCAT(A5," : ",B5)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid"/>
+    <tableColumn id="5" name="desc:lid"/>
+    <tableColumn id="6" name="note:lid"/>
+    <tableColumn id="7" name="name:ltext"/>
+    <tableColumn id="8" name="desc:ltext"/>
+    <tableColumn id="9" name="note:ltext"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="NewTable22" displayName="NewTable22" ref="A7:I8" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A7:I8" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:1"/>
+    <tableColumn id="2" name="label:label"/>
+    <tableColumn id="3" name="signature:support">
+      <calculatedColumnFormula>_xlfn.CONCAT(A8," : ",B8)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid"/>
+    <tableColumn id="5" name="desc:lid"/>
+    <tableColumn id="6" name="note:lid"/>
+    <tableColumn id="7" name="name:ltext"/>
+    <tableColumn id="8" name="desc:ltext"/>
+    <tableColumn id="9" name="note:ltext"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="table_base" displayName="table_base" ref="A2:J3" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A2:J3" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="10">
@@ -1144,7 +1205,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="table_ext" displayName="table_ext" ref="A5:I6" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A5:I6" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="9">
@@ -1424,8 +1485,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1453,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:2">
@@ -1476,17 +1537,224 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7"/>
+  <cols>
+    <col min="1" max="1" width="10.7142857142857" customWidth="1"/>
+    <col min="2" max="3" width="25.7142857142857" customWidth="1"/>
+    <col min="4" max="6" width="10.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="25.7142857142857" customWidth="1"/>
+    <col min="8" max="9" width="50.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT(A2," : ",B2)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xlfn.CONCAT(A5," : ",B5)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="str">
+        <f>_xlfn.CONCAT(A8," : ",B8)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="10.7142857142857" style="1" customWidth="1"/>
-    <col min="2" max="3" width="25.7142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7142857142857" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7142857142857" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="6" width="10.7142857142857" style="1" customWidth="1"/>
     <col min="7" max="7" width="25.7142857142857" style="1" customWidth="1"/>
     <col min="8" max="9" width="50.7142857142857" style="1" customWidth="1"/>
@@ -1496,34 +1764,34 @@
   <sheetData>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1531,29 +1799,29 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>_xlfn.CONCAT(A3," : ",B3)</f>
         <v>0 : ENTITY_</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>19</v>
@@ -1561,31 +1829,31 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1593,29 +1861,29 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>_xlfn.CONCAT(A6," : ",B6)</f>
         <v>0 : ENTITY_</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: dist\data_designer.xaml - support for recent changes. Code cleanup.
</commit_message>
<xml_diff>
--- a/dist/origin.xlsx
+++ b/dist/origin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12045" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="27945" windowHeight="12045" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="@core" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="20">
   <si>
     <t>Settings</t>
   </si>
@@ -40,6 +40,9 @@
     <t>show_support_columns</t>
   </si>
   <si>
+    <t>id:6</t>
+  </si>
+  <si>
     <t>id:1</t>
   </si>
   <si>
@@ -83,9 +86,6 @@
   </si>
   <si>
     <t>type:ref</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>0 : ENTITY_</t>
@@ -717,9 +717,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" quotePrefix="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1107,7 +1104,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="locale" displayName="locale" ref="B9:B10" insertRow="1" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="B9:B10" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="id:1"/>
+    <tableColumn id="1" name="id:6"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1486,7 +1483,7 @@
   <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1540,8 +1537,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7"/>
@@ -1555,31 +1552,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1587,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT(A2," : ",B2)</f>
@@ -1603,42 +1600,42 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1646,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.CONCAT(A5," : ",B5)</f>
@@ -1662,42 +1659,42 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1705,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.CONCAT(A8," : ",B8)</f>
@@ -1721,13 +1718,13 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1746,8 +1743,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
@@ -1764,34 +1761,34 @@
   <sheetData>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1799,29 +1796,29 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>_xlfn.CONCAT(A3," : ",B3)</f>
         <v>0 : ENTITY_</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>19</v>
@@ -1829,31 +1826,31 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1861,29 +1858,29 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>_xlfn.CONCAT(A6," : ",B6)</f>
         <v>0 : ENTITY_</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addin: dist\data_designer.xaml - support json type with validation.
</commit_message>
<xml_diff>
--- a/dist/origin.xlsx
+++ b/dist/origin.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12045" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="27945" windowHeight="11835" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="@core" sheetId="4" r:id="rId1"/>
-    <sheet name="NewTable" sheetId="7" r:id="rId2"/>
-    <sheet name="@examples" sheetId="3" r:id="rId3"/>
+    <sheet name="@examples" sheetId="3" r:id="rId2"/>
+    <sheet name="NewTable" sheetId="7" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -28,8 +31,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
   <si>
     <t>Settings</t>
   </si>
@@ -49,46 +74,55 @@
     <t>label:label</t>
   </si>
   <si>
+    <t>sig:support</t>
+  </si>
+  <si>
+    <t>name:lid</t>
+  </si>
+  <si>
+    <t>desc:lid</t>
+  </si>
+  <si>
+    <t>note:lid</t>
+  </si>
+  <si>
+    <t>name:ltext</t>
+  </si>
+  <si>
+    <t>desc:ltext</t>
+  </si>
+  <si>
+    <t>note:ltext</t>
+  </si>
+  <si>
+    <t>type:ref</t>
+  </si>
+  <si>
+    <t>ENTITY_</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>0 : ENTITY_</t>
+  </si>
+  <si>
+    <t>modifiers:json</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>{"id_0": 25}</t>
+  </si>
+  <si>
     <t>signature:support</t>
-  </si>
-  <si>
-    <t>name:lid</t>
-  </si>
-  <si>
-    <t>desc:lid</t>
-  </si>
-  <si>
-    <t>note:lid</t>
-  </si>
-  <si>
-    <t>name:ltext</t>
-  </si>
-  <si>
-    <t>desc:ltext</t>
-  </si>
-  <si>
-    <t>note:ltext</t>
-  </si>
-  <si>
-    <t>ENTITY_</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>sig:support</t>
-  </si>
-  <si>
-    <t>type:ref</t>
-  </si>
-  <si>
-    <t>0 : ENTITY_</t>
   </si>
 </sst>
 </file>
@@ -704,11 +738,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -769,7 +806,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="37">
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -877,6 +914,12 @@
         <patternFill patternType="none"/>
       </fill>
       <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -1071,25 +1114,25 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="24"/>
-      <tableStyleElement type="headerRow" dxfId="23"/>
-      <tableStyleElement type="totalRow" dxfId="22"/>
-      <tableStyleElement type="firstColumn" dxfId="21"/>
-      <tableStyleElement type="lastColumn" dxfId="20"/>
-      <tableStyleElement type="firstRowStripe" dxfId="19"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="18"/>
+      <tableStyleElement type="wholeTable" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
+      <tableStyleElement type="totalRow" dxfId="24"/>
+      <tableStyleElement type="firstColumn" dxfId="23"/>
+      <tableStyleElement type="lastColumn" dxfId="22"/>
+      <tableStyleElement type="firstRowStripe" dxfId="21"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="20"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="34"/>
-      <tableStyleElement type="totalRow" dxfId="33"/>
-      <tableStyleElement type="firstRowStripe" dxfId="32"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="31"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="30"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="29"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="28"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="27"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="26"/>
-      <tableStyleElement type="pageFieldValues" dxfId="25"/>
+      <tableStyleElement type="headerRow" dxfId="36"/>
+      <tableStyleElement type="totalRow" dxfId="35"/>
+      <tableStyleElement type="firstRowStripe" dxfId="34"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="33"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="32"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="31"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="30"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="29"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="28"/>
+      <tableStyleElement type="pageFieldValues" dxfId="27"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1098,6 +1141,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="@core"/>
+      <sheetName val="@examples"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="ValidateJSON"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1122,66 +1183,6 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="NewTable" displayName="NewTable" ref="A1:I2" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I2" etc:filterBottomFollowUsedRange="0"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="id:1"/>
-    <tableColumn id="2" name="label:label"/>
-    <tableColumn id="3" name="signature:support">
-      <calculatedColumnFormula>_xlfn.CONCAT(A2," : ",B2)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" name="name:lid"/>
-    <tableColumn id="5" name="desc:lid"/>
-    <tableColumn id="6" name="note:lid"/>
-    <tableColumn id="7" name="name:ltext"/>
-    <tableColumn id="8" name="desc:ltext"/>
-    <tableColumn id="9" name="note:ltext"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="NewTabley" displayName="NewTabley" ref="A4:I5" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A4:I5" etc:filterBottomFollowUsedRange="0"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="id:1"/>
-    <tableColumn id="2" name="label:label"/>
-    <tableColumn id="3" name="signature:support">
-      <calculatedColumnFormula>_xlfn.CONCAT(A5," : ",B5)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" name="name:lid"/>
-    <tableColumn id="5" name="desc:lid"/>
-    <tableColumn id="6" name="note:lid"/>
-    <tableColumn id="7" name="name:ltext"/>
-    <tableColumn id="8" name="desc:ltext"/>
-    <tableColumn id="9" name="note:ltext"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="NewTable22" displayName="NewTable22" ref="A7:I8" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A7:I8" etc:filterBottomFollowUsedRange="0"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="id:1"/>
-    <tableColumn id="2" name="label:label"/>
-    <tableColumn id="3" name="signature:support">
-      <calculatedColumnFormula>_xlfn.CONCAT(A8," : ",B8)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" name="name:lid"/>
-    <tableColumn id="5" name="desc:lid"/>
-    <tableColumn id="6" name="note:lid"/>
-    <tableColumn id="7" name="name:ltext"/>
-    <tableColumn id="8" name="desc:ltext"/>
-    <tableColumn id="9" name="note:ltext"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="table_base" displayName="table_base" ref="A2:J3" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A2:J3" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="10">
@@ -1202,10 +1203,10 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="table_ext" displayName="table_ext" ref="A5:I6" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A5:I6" etc:filterBottomFollowUsedRange="0"/>
-  <tableColumns count="9">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="table_ext" displayName="table_ext" ref="A5:K6" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A5:K6" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="id:1" dataDxfId="9"/>
     <tableColumn id="2" name="label:label" dataDxfId="10"/>
     <tableColumn id="3" name="sig:support" dataDxfId="11">
@@ -1217,6 +1218,68 @@
     <tableColumn id="7" name="name:ltext" dataDxfId="15"/>
     <tableColumn id="8" name="desc:ltext" dataDxfId="16"/>
     <tableColumn id="9" name="note:ltext" dataDxfId="17"/>
+    <tableColumn id="10" name="modifiers:json" dataDxfId="18"/>
+    <tableColumn id="11" name="Column1" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="NewTable" displayName="NewTable" ref="A1:I2" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I2" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:1"/>
+    <tableColumn id="2" name="label:label"/>
+    <tableColumn id="3" name="signature:support">
+      <calculatedColumnFormula>_xlfn.CONCAT(A2," : ",B2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid"/>
+    <tableColumn id="5" name="desc:lid"/>
+    <tableColumn id="6" name="note:lid"/>
+    <tableColumn id="7" name="name:ltext"/>
+    <tableColumn id="8" name="desc:ltext"/>
+    <tableColumn id="9" name="note:ltext"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="NewTabley" displayName="NewTabley" ref="A4:I5" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A4:I5" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:1"/>
+    <tableColumn id="2" name="label:label"/>
+    <tableColumn id="3" name="signature:support">
+      <calculatedColumnFormula>_xlfn.CONCAT(A5," : ",B5)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid"/>
+    <tableColumn id="5" name="desc:lid"/>
+    <tableColumn id="6" name="note:lid"/>
+    <tableColumn id="7" name="name:ltext"/>
+    <tableColumn id="8" name="desc:ltext"/>
+    <tableColumn id="9" name="note:ltext"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="NewTable22" displayName="NewTable22" ref="A7:I8" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A7:I8" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:1"/>
+    <tableColumn id="2" name="label:label"/>
+    <tableColumn id="3" name="signature:support">
+      <calculatedColumnFormula>_xlfn.CONCAT(A8," : ",B8)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid"/>
+    <tableColumn id="5" name="desc:lid"/>
+    <tableColumn id="6" name="note:lid"/>
+    <tableColumn id="7" name="name:ltext"/>
+    <tableColumn id="8" name="desc:ltext"/>
+    <tableColumn id="9" name="note:ltext"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1493,10 +1556,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" t="s">
@@ -1507,10 +1570,10 @@
       </c>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="3" t="b">
+      <c r="B4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="b">
+      <c r="C4" s="4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1533,6 +1596,179 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A2:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
+  <cols>
+    <col min="1" max="1" width="10.7142857142857" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7142857142857" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7142857142857" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="10.7142857142857" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7142857142857" style="1" customWidth="1"/>
+    <col min="8" max="9" width="50.7142857142857" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.5714285714286" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>_xlfn.CONCAT(A3," : ",B3)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f>_xlfn.CONCAT(A6," : ",B6)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="2" t="str" cm="1">
+        <f t="array" ref="K6">[1]!ValidateJSON(J6,$A$3:$A$3)</f>
+        <v>Invalid JSON format</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3">
+      <formula1>$C$6:$C$6</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I8"/>
@@ -1558,7 +1794,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -1584,7 +1820,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT(A2," : ",B2)</f>
@@ -1600,13 +1836,13 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1617,7 +1853,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1643,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.CONCAT(A5," : ",B5)</f>
@@ -1659,13 +1895,13 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1676,7 +1912,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -1702,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.CONCAT(A8," : ",B8)</f>
@@ -1718,13 +1954,13 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1736,164 +1972,4 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:J6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
-  <cols>
-    <col min="1" max="1" width="10.7142857142857" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7142857142857" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7142857142857" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="10.7142857142857" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.7142857142857" style="1" customWidth="1"/>
-    <col min="8" max="9" width="50.7142857142857" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.7142857142857" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.14285714285714" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <f>_xlfn.CONCAT(A3," : ",B3)</f>
-        <v>0 : ENTITY_</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="str">
-        <f>_xlfn.CONCAT(A6," : ",B6)</f>
-        <v>0 : ENTITY_</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3">
-      <formula1>$C$6:$C$6</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add: dist\data-designer.xmlm - Contains Display Module for controlling the display of columns with service information.
</commit_message>
<xml_diff>
--- a/dist/origin.xlsx
+++ b/dist/origin.xlsx
@@ -4,16 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="11835" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="27945" windowHeight="12045" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="@core" sheetId="4" r:id="rId1"/>
     <sheet name="@examples" sheetId="3" r:id="rId2"/>
     <sheet name="NewTable" sheetId="7" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,30 +28,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="30">
   <si>
     <t>Settings</t>
   </si>
@@ -65,7 +40,7 @@
     <t>show_support_columns</t>
   </si>
   <si>
-    <t>id:6</t>
+    <t>id:24</t>
   </si>
   <si>
     <t>id:1</t>
@@ -98,6 +73,9 @@
     <t>type:ref</t>
   </si>
   <si>
+    <t>r</t>
+  </si>
+  <si>
     <t>ENTITY_</t>
   </si>
   <si>
@@ -116,13 +94,31 @@
     <t>modifiers:json</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>{"id_0": 25}</t>
+    <t>{"Entry_0":["0","5557"]}</t>
+  </si>
+  <si>
+    <t>id:7</t>
   </si>
   <si>
     <t>signature:support</t>
+  </si>
+  <si>
+    <t>ENTITY_1</t>
+  </si>
+  <si>
+    <t>ENTITY_2</t>
+  </si>
+  <si>
+    <t>ENTITY_3</t>
+  </si>
+  <si>
+    <t>ENTITY_4</t>
+  </si>
+  <si>
+    <t>ENTITY_5</t>
+  </si>
+  <si>
+    <t>ENTITY_6</t>
   </si>
 </sst>
 </file>
@@ -806,7 +802,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="45">
     <dxf>
       <fill>
         <patternFill patternType="none"/>
@@ -919,7 +915,58 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <alignment vertical="center"/>
     </dxf>
     <dxf>
       <fill>
@@ -1114,25 +1161,25 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="26"/>
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="totalRow" dxfId="24"/>
-      <tableStyleElement type="firstColumn" dxfId="23"/>
-      <tableStyleElement type="lastColumn" dxfId="22"/>
-      <tableStyleElement type="firstRowStripe" dxfId="21"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="20"/>
+      <tableStyleElement type="wholeTable" dxfId="34"/>
+      <tableStyleElement type="headerRow" dxfId="33"/>
+      <tableStyleElement type="totalRow" dxfId="32"/>
+      <tableStyleElement type="firstColumn" dxfId="31"/>
+      <tableStyleElement type="lastColumn" dxfId="30"/>
+      <tableStyleElement type="firstRowStripe" dxfId="29"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="28"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="36"/>
-      <tableStyleElement type="totalRow" dxfId="35"/>
-      <tableStyleElement type="firstRowStripe" dxfId="34"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="33"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="32"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="31"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="30"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="29"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="28"/>
-      <tableStyleElement type="pageFieldValues" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="44"/>
+      <tableStyleElement type="totalRow" dxfId="43"/>
+      <tableStyleElement type="firstRowStripe" dxfId="42"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="41"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="40"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="39"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="38"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="37"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="36"/>
+      <tableStyleElement type="pageFieldValues" dxfId="35"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1143,29 +1190,11 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="@core"/>
-      <sheetName val="@examples"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="ValidateJSON"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="locale" displayName="locale" ref="B9:B10" insertRow="1" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="B9:B10" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="id:6"/>
+    <tableColumn id="1" name="id:24"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1204,9 +1233,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="table_ext" displayName="table_ext" ref="A5:K6" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A5:K6" etc:filterBottomFollowUsedRange="0"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="table_ext" displayName="table_ext" ref="A5:J6" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A5:J6" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="10">
     <tableColumn id="1" name="id:1" dataDxfId="9"/>
     <tableColumn id="2" name="label:label" dataDxfId="10"/>
     <tableColumn id="3" name="sig:support" dataDxfId="11">
@@ -1219,13 +1248,32 @@
     <tableColumn id="8" name="desc:ltext" dataDxfId="16"/>
     <tableColumn id="9" name="note:ltext" dataDxfId="17"/>
     <tableColumn id="10" name="modifiers:json" dataDxfId="18"/>
-    <tableColumn id="11" name="Column1" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="modifiers" displayName="modifiers" ref="A8:I15" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A8:I15" etc:filterBottomFollowUsedRange="0"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="id:7" dataDxfId="19"/>
+    <tableColumn id="2" name="label:label" dataDxfId="20"/>
+    <tableColumn id="3" name="signature:support" dataDxfId="21">
+      <calculatedColumnFormula>_xlfn.CONCAT(A9," : ",B9)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="name:lid" dataDxfId="22"/>
+    <tableColumn id="5" name="desc:lid" dataDxfId="23"/>
+    <tableColumn id="6" name="note:lid" dataDxfId="24"/>
+    <tableColumn id="7" name="name:ltext" dataDxfId="25"/>
+    <tableColumn id="8" name="desc:ltext" dataDxfId="26"/>
+    <tableColumn id="9" name="note:ltext" dataDxfId="27"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStylePreset3_Accent1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="NewTable" displayName="NewTable" ref="A1:I2" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:I2" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="9">
@@ -1245,7 +1293,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="NewTabley" displayName="NewTabley" ref="A4:I5" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A4:I5" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="9">
@@ -1265,7 +1313,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="NewTable22" displayName="NewTable22" ref="A7:I8" totalsRowShown="0">
   <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A7:I8" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="9">
@@ -1546,7 +1594,7 @@
   <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1571,7 +1619,7 @@
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
@@ -1598,18 +1646,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:K6"/>
+  <dimension ref="A2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7142857142857" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.7142857142857" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.7142857142857" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="10.7142857142857" style="1" customWidth="1"/>
+    <col min="4" max="6" width="10.7142857142857" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="25.7142857142857" style="1" customWidth="1"/>
     <col min="8" max="9" width="50.7142857142857" style="1" customWidth="1"/>
     <col min="10" max="10" width="36.5714285714286" style="1" customWidth="1"/>
@@ -1649,15 +1697,15 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="1">
-        <v>0</v>
+      <c r="A3" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>_xlfn.CONCAT(A3," : ",B3)</f>
-        <v>0 : ENTITY_</v>
+        <v>r : ENTITY_</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1669,19 +1717,19 @@
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1710,18 +1758,15 @@
         <v>12</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>_xlfn.CONCAT(A6," : ",B6)</f>
@@ -1737,20 +1782,255 @@
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="2" t="str" cm="1">
-        <f t="array" ref="K6">[1]!ValidateJSON(J6,$A$3:$A$3)</f>
-        <v>Invalid JSON format</v>
+    </row>
+    <row r="8" customHeight="1" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>_xlfn.CONCAT(A9," : ",B9)</f>
+        <v>0 : ENTITY_</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>_xlfn.CONCAT(A10," : ",B10)</f>
+        <v>1 : ENTITY_1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>_xlfn.CONCAT(A11," : ",B11)</f>
+        <v>2 : ENTITY_2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1">
+        <v>11</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>_xlfn.CONCAT(A12," : ",B12)</f>
+        <v>3 : ENTITY_3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>_xlfn.CONCAT(A13," : ",B13)</f>
+        <v>4 : ENTITY_4</v>
+      </c>
+      <c r="D13" s="1">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1">
+        <v>17</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>_xlfn.CONCAT(A14," : ",B14)</f>
+        <v>5 : ENTITY_5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>18</v>
+      </c>
+      <c r="E14" s="1">
+        <v>19</v>
+      </c>
+      <c r="F14" s="1">
+        <v>20</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>_xlfn.CONCAT(A15," : ",B15)</f>
+        <v>6 : ENTITY_6</v>
+      </c>
+      <c r="D15" s="1">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1">
+        <v>22</v>
+      </c>
+      <c r="F15" s="1">
+        <v>23</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1761,9 +2041,10 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1774,14 +2055,15 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="10.7142857142857" customWidth="1"/>
-    <col min="2" max="3" width="25.7142857142857" customWidth="1"/>
-    <col min="4" max="6" width="10.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="25.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="25.7142857142857" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="10.7142857142857" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="25.7142857142857" customWidth="1"/>
     <col min="8" max="9" width="50.7142857142857" customWidth="1"/>
   </cols>
@@ -1794,7 +2076,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -1820,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT(A2," : ",B2)</f>
@@ -1836,13 +2118,13 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1853,7 +2135,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1879,7 +2161,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.CONCAT(A5," : ",B5)</f>
@@ -1895,13 +2177,13 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1912,7 +2194,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -1938,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.CONCAT(A8," : ",B8)</f>
@@ -1954,13 +2236,13 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>